<commit_message>
finished logic for EmptyWellFinder.py
</commit_message>
<xml_diff>
--- a/app/demo_platemap.xlsx
+++ b/app/demo_platemap.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markg\samplesheetApp\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markg\SheetApp\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDB107FF-1172-425E-A885-251AAB86EB45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B893CE4-3888-44FA-91A2-F20C19B119C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-10990" yWindow="-21710" windowWidth="38620" windowHeight="21100" xr2:uid="{5957B19C-9D83-AD4C-BF7B-C8A84381153B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{5957B19C-9D83-AD4C-BF7B-C8A84381153B}"/>
   </bookViews>
   <sheets>
     <sheet name="SMARTseq2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t xml:space="preserve">Experiment Name: </t>
   </si>
@@ -98,9 +98,6 @@
     <t>All samples are from single cells and should be uniquely indexed before pooling and sequencing</t>
   </si>
   <si>
-    <t>A1</t>
-  </si>
-  <si>
     <t>A2</t>
   </si>
   <si>
@@ -176,9 +173,6 @@
     <t>C2</t>
   </si>
   <si>
-    <t>C3</t>
-  </si>
-  <si>
     <t>C4</t>
   </si>
   <si>
@@ -197,9 +191,6 @@
     <t>C9</t>
   </si>
   <si>
-    <t>C10</t>
-  </si>
-  <si>
     <t>C11</t>
   </si>
   <si>
@@ -311,18 +302,6 @@
     <t>F12</t>
   </si>
   <si>
-    <t>G1</t>
-  </si>
-  <si>
-    <t>G2</t>
-  </si>
-  <si>
-    <t>G3</t>
-  </si>
-  <si>
-    <t>G4</t>
-  </si>
-  <si>
     <t>G5</t>
   </si>
   <si>
@@ -380,10 +359,19 @@
     <t>H11</t>
   </si>
   <si>
-    <t>H12</t>
-  </si>
-  <si>
-    <t>E6</t>
+    <t>Water</t>
+  </si>
+  <si>
+    <t>water</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  water</t>
+  </si>
+  <si>
+    <t>wat   er</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wAter   </t>
   </si>
 </sst>
 </file>
@@ -819,16 +807,16 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
   <cols>
-    <col min="1" max="1" width="16.8984375" customWidth="1"/>
-    <col min="2" max="13" width="14.8984375" customWidth="1"/>
+    <col min="1" max="1" width="16.875" customWidth="1"/>
+    <col min="2" max="13" width="14.875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +824,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -844,7 +832,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -852,7 +840,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -860,7 +848,7 @@
         <v>45406</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -868,7 +856,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -876,11 +864,11 @@
         <v>18</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="3"/>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
       <c r="B8" s="7">
         <v>1</v>
       </c>
@@ -918,430 +906,422 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A9" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="2"/>
+      <c r="C9" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="F9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="2" t="s">
+      <c r="H9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="I9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>30</v>
-      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A10" s="8" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="M10" s="2" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A11" s="8" t="s">
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="K11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>54</v>
-      </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="K12" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A13" s="8" t="s">
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="G13" s="2"/>
+      <c r="H13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="K13" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A14" s="8" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="K14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>89</v>
-      </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A15" s="8" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="I15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="E15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="K15" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="L15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>101</v>
-      </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A16" s="8" t="s">
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="I16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="F16" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="K16" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="L16" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="M16" s="2" t="s">
-        <v>113</v>
-      </c>
+      <c r="M16" s="2"/>
     </row>
-    <row r="19" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="20" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="21" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="22" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="23" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="24" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="25" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="26" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="27" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="28" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="29" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="30" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="31" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="32" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="33" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="34" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="35" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="36" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="37" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="38" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="39" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="40" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="41" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="42" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="43" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="44" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="45" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="46" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="47" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="48" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="49" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="50" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="51" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="52" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="53" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="54" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="55" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="56" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="57" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="58" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="59" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="60" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="61" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="62" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="63" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="64" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="65" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="66" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="67" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="68" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="69" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="70" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="71" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="72" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="73" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="74" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="75" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="76" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="77" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="78" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="79" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="80" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="81" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="82" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="83" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="84" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="85" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="86" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="87" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="88" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="89" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="97" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="98" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="99" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="100" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="101" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="102" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="103" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="104" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="105" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="106" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="107" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="111" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="112" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="113" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="114" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="127" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="128" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="129" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="130" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="131" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="145" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="146" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="147" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="148" customFormat="1" x14ac:dyDescent="0.3"/>
-    <row r="149" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="25" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="26" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="27" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="28" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="29" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="30" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="31" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="32" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="33" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="34" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="35" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="36" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="37" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="38" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="39" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="40" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="41" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="42" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="43" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="44" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="45" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="46" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="47" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="48" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="49" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="50" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="51" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="52" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="53" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="54" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="55" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="56" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="57" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="58" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="59" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="60" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="61" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="62" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="63" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="64" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="65" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="66" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="67" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="68" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="69" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="70" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="71" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="72" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="73" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="74" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="75" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="76" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="77" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="78" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="79" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="80" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="81" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="82" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="83" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="84" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="85" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="86" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="87" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="88" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="89" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="97" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="98" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="99" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="100" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="101" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="102" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="103" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="104" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="105" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="106" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="107" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="111" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="112" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="113" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="114" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="127" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="128" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="129" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="130" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="131" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="145" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="146" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="147" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="148" customFormat="1" x14ac:dyDescent="0.5"/>
+    <row r="149" customFormat="1" x14ac:dyDescent="0.5"/>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added code to parse input file for SS2
</commit_message>
<xml_diff>
--- a/app/demo_platemap.xlsx
+++ b/app/demo_platemap.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\markg\SheetApp\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B893CE4-3888-44FA-91A2-F20C19B119C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51CDCFE0-1831-4EED-89D5-A90CCFDBAEFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{5957B19C-9D83-AD4C-BF7B-C8A84381153B}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="11422" xr2:uid="{5957B19C-9D83-AD4C-BF7B-C8A84381153B}"/>
   </bookViews>
   <sheets>
     <sheet name="SMARTseq2" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="114">
   <si>
     <t xml:space="preserve">Experiment Name: </t>
   </si>
@@ -113,9 +113,6 @@
     <t>A6</t>
   </si>
   <si>
-    <t>A7</t>
-  </si>
-  <si>
     <t>A8</t>
   </si>
   <si>
@@ -359,19 +356,31 @@
     <t>H11</t>
   </si>
   <si>
-    <t>Water</t>
-  </si>
-  <si>
     <t>water</t>
   </si>
   <si>
-    <t xml:space="preserve">  water</t>
-  </si>
-  <si>
-    <t>wat   er</t>
-  </si>
-  <si>
-    <t xml:space="preserve">wAter   </t>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>G2</t>
+  </si>
+  <si>
+    <t>G4</t>
+  </si>
+  <si>
+    <t>H12</t>
+  </si>
+  <si>
+    <t>E6</t>
+  </si>
+  <si>
+    <t>C10</t>
+  </si>
+  <si>
+    <t>G3</t>
   </si>
 </sst>
 </file>
@@ -807,7 +816,7 @@
   <dimension ref="A1:M149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.5"/>
@@ -927,22 +936,22 @@
         <v>23</v>
       </c>
       <c r="H9" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="I9" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="I9" s="2" t="s">
+      <c r="J9" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="2" t="s">
+      <c r="K9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="L9" s="2" t="s">
+      <c r="M9" s="2" t="s">
         <v>28</v>
-      </c>
-      <c r="M9" s="2" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
@@ -950,40 +959,40 @@
         <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="E10" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="I10" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="I10" s="2" t="s">
+      <c r="J10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J10" s="2" t="s">
+      <c r="K10" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="L10" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="L10" s="2" t="s">
+      <c r="M10" s="2" t="s">
         <v>40</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.5">
@@ -991,38 +1000,40 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="H11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="I11" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="J11" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="L11" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="K11" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="L11" s="2" t="s">
+      <c r="M11" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
@@ -1030,40 +1041,40 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="D12" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="E12" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="F12" s="2" t="s">
+      <c r="G12" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H12" s="2" t="s">
+      <c r="I12" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="J12" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="2" t="s">
+      <c r="L12" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L12" s="2" t="s">
+      <c r="M12" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="M12" s="2" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
@@ -1071,38 +1082,40 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="D13" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="E13" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="G13" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="J13" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="K13" s="2" t="s">
+      <c r="L13" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="L13" s="2" t="s">
+      <c r="M13" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.5">
@@ -1110,40 +1123,40 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C14" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="E14" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G14" s="2" t="s">
+      <c r="H14" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="H14" s="2" t="s">
+      <c r="I14" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="J14" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="J14" s="2" t="s">
+      <c r="K14" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K14" s="2" t="s">
+      <c r="L14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="L14" s="2" t="s">
+      <c r="M14" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
@@ -1151,40 +1164,40 @@
         <v>13</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>107</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>109</v>
       </c>
       <c r="F15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G15" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="G15" s="2" t="s">
+      <c r="H15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="H15" s="2" t="s">
+      <c r="I15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="I15" s="2" t="s">
+      <c r="J15" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="J15" s="2" t="s">
+      <c r="K15" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="L15" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="L15" s="2" t="s">
+      <c r="M15" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
@@ -1192,39 +1205,41 @@
         <v>14</v>
       </c>
       <c r="B16" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="F16" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F16" s="2" t="s">
+      <c r="G16" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="G16" s="2" t="s">
+      <c r="H16" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="H16" s="2" t="s">
+      <c r="I16" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="J16" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="J16" s="2" t="s">
+      <c r="K16" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="L16" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="L16" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="M16" s="2"/>
+      <c r="M16" s="2" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="19" customFormat="1" x14ac:dyDescent="0.5"/>
     <row r="20" customFormat="1" x14ac:dyDescent="0.5"/>
@@ -1330,14 +1345,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="294672bb-f7e7-4211-b002-83a34d9eceab" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="285b1053-35af-46c5-a010-8e24eac673b3">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1536,21 +1549,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="294672bb-f7e7-4211-b002-83a34d9eceab" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="285b1053-35af-46c5-a010-8e24eac673b3">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFC10D2-79B4-43D6-916F-A60F8E7C48F3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B798312-2A8D-409A-9800-62D488A2EFC3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="294672bb-f7e7-4211-b002-83a34d9eceab"/>
-    <ds:schemaRef ds:uri="285b1053-35af-46c5-a010-8e24eac673b3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1575,9 +1587,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3B798312-2A8D-409A-9800-62D488A2EFC3}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0EFC10D2-79B4-43D6-916F-A60F8E7C48F3}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="294672bb-f7e7-4211-b002-83a34d9eceab"/>
+    <ds:schemaRef ds:uri="285b1053-35af-46c5-a010-8e24eac673b3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>